<commit_message>
Bo so do Activity, chi ve so do tuan tu
</commit_message>
<xml_diff>
--- a/BangKeHoachLamViecNhom.xlsx
+++ b/BangKeHoachLamViecNhom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>STT</t>
   </si>
@@ -114,9 +114,6 @@
     <t>UseCase</t>
   </si>
   <si>
-    <t>Activity Diagram</t>
-  </si>
-  <si>
     <t>Đặc tả UseCasse</t>
   </si>
   <si>
@@ -169,9 +166,6 @@
   </si>
   <si>
     <t>Viết đặc tả cho từng UseCase</t>
-  </si>
-  <si>
-    <t>Phân tích thiết kế Activity Diagram</t>
   </si>
   <si>
     <t>Phân tích thiết kế sơ đồ tuần tự</t>
@@ -1028,7 +1022,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1038,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="38" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="38" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1207,7 +1201,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="29" t="s">
         <v>21</v>
@@ -1230,7 +1224,7 @@
       <c r="A5" s="46"/>
       <c r="B5" s="35"/>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>21</v>
@@ -1253,7 +1247,7 @@
       <c r="A6" s="46"/>
       <c r="B6" s="35"/>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>22</v>
@@ -1276,7 +1270,7 @@
       <c r="A7" s="46"/>
       <c r="B7" s="35"/>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>22</v>
@@ -1299,7 +1293,7 @@
       <c r="A8" s="47"/>
       <c r="B8" s="36"/>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>22</v>
@@ -1326,7 +1320,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="30" t="s">
         <v>23</v>
@@ -1353,10 +1347,10 @@
         <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="10"/>
@@ -1376,10 +1370,10 @@
       <c r="A11" s="32"/>
       <c r="B11" s="35"/>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="10"/>
@@ -1399,7 +1393,7 @@
       <c r="A12" s="32"/>
       <c r="B12" s="35"/>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="30" t="s">
         <v>21</v>
@@ -1422,7 +1416,7 @@
       <c r="A13" s="32"/>
       <c r="B13" s="35"/>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="30" t="s">
         <v>21</v>
@@ -1445,10 +1439,10 @@
       <c r="A14" s="33"/>
       <c r="B14" s="36"/>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="10"/>
@@ -1472,10 +1466,10 @@
         <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -1499,10 +1493,10 @@
         <v>29</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
@@ -1526,7 +1520,7 @@
         <v>30</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D17" s="30" t="s">
         <v>23</v>
@@ -1550,10 +1544,10 @@
         <v>7</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="27" t="s">
         <v>22</v>
@@ -1577,26 +1571,26 @@
         <v>8</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
+      <c r="I19" s="20"/>
       <c r="J19" s="24"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="20"/>
       <c r="M19" s="24"/>
       <c r="N19" s="20"/>
       <c r="O19" s="24"/>
-      <c r="P19" s="20"/>
+      <c r="P19" s="24"/>
       <c r="Q19" s="24"/>
     </row>
     <row r="20" spans="1:17" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1607,14 +1601,14 @@
         <v>33</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>54</v>
       </c>
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
-      <c r="G20" s="20"/>
+      <c r="G20" s="24"/>
       <c r="H20" s="24"/>
       <c r="I20" s="20"/>
       <c r="J20" s="24"/>
@@ -1626,34 +1620,10 @@
       <c r="P20" s="24"/>
       <c r="Q20" s="24"/>
     </row>
-    <row r="21" spans="1:17" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22">
-        <v>10</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-    </row>
-    <row r="22" spans="1:17" ht="40.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:17" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="16"/>
+    </row>
+    <row r="22" spans="1:17" ht="40.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="16"/>
     </row>
     <row r="23" spans="1:17" ht="26.45" customHeight="1" x14ac:dyDescent="0.35">
@@ -1662,21 +1632,19 @@
     <row r="24" spans="1:17" ht="30.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="16"/>
     </row>
-    <row r="25" spans="1:17" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="16"/>
-    </row>
+    <row r="25" spans="1:17" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:17" ht="34.9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:17" ht="48" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:17" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:17" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="17"/>
+    </row>
     <row r="29" spans="1:17" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="17"/>
     </row>
     <row r="30" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
     </row>
-    <row r="31" spans="1:17" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="17"/>
-    </row>
+    <row r="31" spans="1:17" ht="33.6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:17" ht="37.9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="18:18" ht="37.9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="18:18" ht="37.15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Cap nhat phan cong cong viec tuan 11
</commit_message>
<xml_diff>
--- a/BangKeHoachLamViecNhom.xlsx
+++ b/BangKeHoachLamViecNhom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
   <si>
     <t>STT</t>
   </si>
@@ -184,6 +184,18 @@
   </si>
   <si>
     <t>Nguyễn Bùi Thiên Đạt, Lý Gia Đào</t>
+  </si>
+  <si>
+    <t>Trần Văn Đồng, Trần Quang Đạo,Nguyễn Bùi Thiên Đạt,Lý Gia Đào</t>
+  </si>
+  <si>
+    <t>Nguyễn Bùi Thiên Đạt, Lý Gia Đào, Trần Văn Đồng,Trần Quang Đạo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Trần Quang Đạo,Nguyễn Bùi Thiên Đạt</t>
+  </si>
+  <si>
+    <t>Nguyễn Bùi Thiên Đạt, Trần Văn Đồng</t>
   </si>
 </sst>
 </file>
@@ -1022,7 +1034,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1032,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="38" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="38" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1469,7 +1481,7 @@
         <v>45</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -1485,7 +1497,7 @@
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
     </row>
-    <row r="16" spans="1:46" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>5</v>
       </c>
@@ -1496,7 +1508,7 @@
         <v>46</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
@@ -1523,7 +1535,7 @@
         <v>47</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
@@ -1550,7 +1562,7 @@
         <v>48</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="E18" s="24"/>
       <c r="F18" s="25"/>
@@ -1584,7 +1596,7 @@
       <c r="G19" s="20"/>
       <c r="H19" s="24"/>
       <c r="I19" s="20"/>
-      <c r="J19" s="24"/>
+      <c r="J19" s="10"/>
       <c r="K19" s="24"/>
       <c r="L19" s="20"/>
       <c r="M19" s="24"/>

</xml_diff>

<commit_message>
phan chia cong viec tuan 12
</commit_message>
<xml_diff>
--- a/BangKeHoachLamViecNhom.xlsx
+++ b/BangKeHoachLamViecNhom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>STT</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Sơ đồ tuần tự</t>
   </si>
   <si>
-    <t>State machine</t>
-  </si>
-  <si>
     <t>Tổng quan của cửa hàng</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>Phân tích thiết kế sơ đồ tuần tự</t>
   </si>
   <si>
-    <t>Phân tích thiết kế state machine</t>
-  </si>
-  <si>
     <t>Trần Văn Đồng, Nguyễn Bùi Thiên Đạt</t>
   </si>
   <si>
@@ -183,9 +177,6 @@
     <t>Trần Văn Đồng, Trần Quang Đạo</t>
   </si>
   <si>
-    <t>Nguyễn Bùi Thiên Đạt, Lý Gia Đào</t>
-  </si>
-  <si>
     <t>Trần Văn Đồng, Trần Quang Đạo,Nguyễn Bùi Thiên Đạt,Lý Gia Đào</t>
   </si>
   <si>
@@ -196,6 +187,12 @@
   </si>
   <si>
     <t>Nguyễn Bùi Thiên Đạt, Trần Văn Đồng</t>
+  </si>
+  <si>
+    <t>ERD</t>
+  </si>
+  <si>
+    <t>Vẽ sơ đồ ERD</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1031,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1044,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="38" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="38" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1213,7 +1210,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="29" t="s">
         <v>21</v>
@@ -1236,7 +1233,7 @@
       <c r="A5" s="46"/>
       <c r="B5" s="35"/>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>21</v>
@@ -1259,7 +1256,7 @@
       <c r="A6" s="46"/>
       <c r="B6" s="35"/>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>22</v>
@@ -1282,7 +1279,7 @@
       <c r="A7" s="46"/>
       <c r="B7" s="35"/>
       <c r="C7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>22</v>
@@ -1305,7 +1302,7 @@
       <c r="A8" s="47"/>
       <c r="B8" s="36"/>
       <c r="C8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>22</v>
@@ -1332,7 +1329,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="30" t="s">
         <v>23</v>
@@ -1359,10 +1356,10 @@
         <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="10"/>
@@ -1382,10 +1379,10 @@
       <c r="A11" s="32"/>
       <c r="B11" s="35"/>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="10"/>
@@ -1405,7 +1402,7 @@
       <c r="A12" s="32"/>
       <c r="B12" s="35"/>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="30" t="s">
         <v>21</v>
@@ -1428,7 +1425,7 @@
       <c r="A13" s="32"/>
       <c r="B13" s="35"/>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="30" t="s">
         <v>21</v>
@@ -1451,10 +1448,10 @@
       <c r="A14" s="33"/>
       <c r="B14" s="36"/>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="10"/>
@@ -1478,10 +1475,10 @@
         <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -1505,10 +1502,10 @@
         <v>29</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
@@ -1532,10 +1529,10 @@
         <v>30</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
@@ -1559,10 +1556,10 @@
         <v>31</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E18" s="24"/>
       <c r="F18" s="25"/>
@@ -1586,10 +1583,10 @@
         <v>32</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
@@ -1610,13 +1607,13 @@
         <v>9</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
@@ -1624,7 +1621,7 @@
       <c r="H20" s="24"/>
       <c r="I20" s="20"/>
       <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
+      <c r="K20" s="10"/>
       <c r="L20" s="20"/>
       <c r="M20" s="24"/>
       <c r="N20" s="20"/>

</xml_diff>

<commit_message>
Update cong viec tuan 12
</commit_message>
<xml_diff>
--- a/BangKeHoachLamViecNhom.xlsx
+++ b/BangKeHoachLamViecNhom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>STT</t>
   </si>
@@ -193,6 +193,27 @@
   </si>
   <si>
     <t>Vẽ sơ đồ ERD</t>
+  </si>
+  <si>
+    <t>Thiết Kế Giao Diện</t>
+  </si>
+  <si>
+    <t>Thiết Kế Dữ Liệu</t>
+  </si>
+  <si>
+    <t>Thiết Kế Xử lý</t>
+  </si>
+  <si>
+    <t>Viết thiết kế giao diện</t>
+  </si>
+  <si>
+    <t>viết thiết thế dữ liệu</t>
+  </si>
+  <si>
+    <t>viết thiết kế xử lý</t>
+  </si>
+  <si>
+    <t>Trần Văn Đồng</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1052,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1041,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="38" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="38" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1617,7 +1638,7 @@
       </c>
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
+      <c r="G20" s="20"/>
       <c r="H20" s="24"/>
       <c r="I20" s="20"/>
       <c r="J20" s="24"/>
@@ -1629,46 +1650,122 @@
       <c r="P20" s="24"/>
       <c r="Q20" s="24"/>
     </row>
-    <row r="21" spans="1:17" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="16"/>
-    </row>
-    <row r="22" spans="1:17" ht="40.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="16"/>
-    </row>
-    <row r="23" spans="1:17" ht="26.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="16"/>
+    <row r="21" spans="1:17" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22">
+        <v>10</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+    </row>
+    <row r="22" spans="1:17" ht="40.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="22">
+        <v>11</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+    </row>
+    <row r="23" spans="1:17" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="22">
+        <v>12</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="28"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
     </row>
     <row r="24" spans="1:17" ht="30.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="16"/>
     </row>
-    <row r="25" spans="1:17" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:17" ht="34.9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:17" ht="48" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:17" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
-    </row>
-    <row r="29" spans="1:17" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="17"/>
-    </row>
-    <row r="30" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
-    </row>
-    <row r="31" spans="1:17" ht="33.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:17" ht="37.9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="18:18" ht="37.9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="18:18" ht="37.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="18:18" ht="31.9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="18:18" ht="43.9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="18:18" ht="34.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="18:18" ht="37.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="18:18" ht="31.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="18:18" ht="37.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="18:18" ht="50.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="18:18" ht="41.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="18:18" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="16"/>
+    </row>
+    <row r="26" spans="1:17" ht="34.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="16"/>
+    </row>
+    <row r="27" spans="1:17" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="16"/>
+    </row>
+    <row r="28" spans="1:17" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:17" ht="36.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:17" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="17"/>
+    </row>
+    <row r="32" spans="1:17" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="17"/>
+    </row>
+    <row r="33" spans="1:18" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="17"/>
+    </row>
+    <row r="34" spans="1:18" ht="37.15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:18" ht="31.9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:18" ht="43.9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:18" ht="34.15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:18" ht="37.15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:18" ht="31.15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:18" ht="37.15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:18" ht="50.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:18" ht="41.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:18" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R43" s="15"/>
     </row>
-    <row r="44" spans="18:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A10:A14"/>

</xml_diff>

<commit_message>
nhom truong phan cong cong viec tuan 13
</commit_message>
<xml_diff>
--- a/BangKeHoachLamViecNhom.xlsx
+++ b/BangKeHoachLamViecNhom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
   <si>
     <t>STT</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Trạng thái</t>
   </si>
   <si>
-    <t>TIMELINE THỰC HIỆN HỆ THỐNG QUẢN LÝ BÁN ĐIỆN THOẠI</t>
-  </si>
-  <si>
     <t>Tháng 10</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>Nguyễn Bùi Thiên Đạt</t>
   </si>
   <si>
-    <t>Lý Gia Đào</t>
-  </si>
-  <si>
     <t>CÔNG VIỆC</t>
   </si>
   <si>
@@ -177,12 +171,6 @@
     <t>Trần Văn Đồng, Trần Quang Đạo</t>
   </si>
   <si>
-    <t>Trần Văn Đồng, Trần Quang Đạo,Nguyễn Bùi Thiên Đạt,Lý Gia Đào</t>
-  </si>
-  <si>
-    <t>Nguyễn Bùi Thiên Đạt, Lý Gia Đào, Trần Văn Đồng,Trần Quang Đạo</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Trần Quang Đạo,Nguyễn Bùi Thiên Đạt</t>
   </si>
   <si>
@@ -207,20 +195,29 @@
     <t>Viết thiết kế giao diện</t>
   </si>
   <si>
-    <t>viết thiết thế dữ liệu</t>
-  </si>
-  <si>
-    <t>viết thiết kế xử lý</t>
-  </si>
-  <si>
     <t>Trần Văn Đồng</t>
+  </si>
+  <si>
+    <t>TIMELINE THỰC HIỆN THIẾT KẾ HỆ THỐNG WEBSITE BÁN ĐIỆN THOẠI</t>
+  </si>
+  <si>
+    <t>Cả nhóm</t>
+  </si>
+  <si>
+    <t>Viết thiết thế dữ liệu</t>
+  </si>
+  <si>
+    <t>Viết thiết kế xử lý</t>
+  </si>
+  <si>
+    <t>Lý Gia Đào Trần Văn Đồng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,12 +248,6 @@
     </font>
     <font>
       <sz val="15"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -618,18 +609,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -641,64 +632,64 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -735,9 +726,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1062,40 +1050,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="38" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="47.42578125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="9" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" style="9" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" style="9" customWidth="1"/>
-    <col min="12" max="12" width="23.7109375" style="9" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" style="9" customWidth="1"/>
-    <col min="14" max="14" width="21.85546875" style="9" customWidth="1"/>
-    <col min="15" max="15" width="22.28515625" style="9" customWidth="1"/>
-    <col min="16" max="16" width="22" style="9" customWidth="1"/>
-    <col min="17" max="17" width="24.7109375" style="9" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" style="9" customWidth="1"/>
-    <col min="19" max="25" width="9.140625" style="9"/>
-    <col min="26" max="26" width="11.28515625" style="9" customWidth="1"/>
-    <col min="27" max="45" width="9.140625" style="9"/>
-    <col min="46" max="46" width="17.7109375" style="9" customWidth="1"/>
-    <col min="47" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="8.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="47.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" style="8" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" style="8" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" style="8" customWidth="1"/>
+    <col min="14" max="14" width="21.85546875" style="8" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" style="8" customWidth="1"/>
+    <col min="16" max="16" width="22" style="8" customWidth="1"/>
+    <col min="17" max="17" width="24.7109375" style="8" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="8" customWidth="1"/>
+    <col min="19" max="25" width="9.140625" style="8"/>
+    <col min="26" max="26" width="11.28515625" style="8" customWidth="1"/>
+    <col min="27" max="45" width="9.140625" style="8"/>
+    <col min="46" max="46" width="17.7109375" style="8" customWidth="1"/>
+    <col min="47" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" ht="61.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -1148,26 +1136,26 @@
         <v>0</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="44"/>
       <c r="D2" s="40" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" s="43"/>
       <c r="G2" s="43"/>
       <c r="H2" s="44"/>
       <c r="I2" s="42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J2" s="43"/>
       <c r="K2" s="43"/>
       <c r="L2" s="44"/>
       <c r="M2" s="42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N2" s="43"/>
       <c r="O2" s="43"/>
@@ -1179,47 +1167,47 @@
     <row r="3" spans="1:46" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
       <c r="B3" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="41"/>
       <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="Q3" s="41"/>
     </row>
@@ -1227,531 +1215,533 @@
       <c r="A4" s="45">
         <v>1</v>
       </c>
-      <c r="B4" s="48" t="s">
-        <v>25</v>
+      <c r="B4" s="47" t="s">
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="12"/>
+        <v>31</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="11"/>
     </row>
     <row r="5" spans="1:46" ht="35.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="35"/>
       <c r="C5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
+        <v>32</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
     </row>
     <row r="6" spans="1:46" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="35"/>
       <c r="C6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
+        <v>33</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
     </row>
     <row r="7" spans="1:46" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="35"/>
       <c r="C7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
+        <v>34</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
     </row>
     <row r="8" spans="1:46" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="36"/>
       <c r="C8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
     </row>
     <row r="9" spans="1:46" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26">
         <v>2</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
+        <v>36</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
     </row>
     <row r="10" spans="1:46" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
         <v>3</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
+        <v>37</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
     </row>
     <row r="11" spans="1:46" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32"/>
       <c r="B11" s="35"/>
       <c r="C11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
     </row>
     <row r="12" spans="1:46" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="32"/>
       <c r="B12" s="35"/>
       <c r="C12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
+        <v>40</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
     </row>
     <row r="13" spans="1:46" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32"/>
       <c r="B13" s="35"/>
       <c r="C13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
+        <v>39</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
     </row>
     <row r="14" spans="1:46" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33"/>
       <c r="B14" s="36"/>
       <c r="C14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+    </row>
+    <row r="15" spans="1:46" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="27">
+        <v>4</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+    </row>
+    <row r="16" spans="1:46" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27">
+        <v>5</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D16" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+    </row>
+    <row r="17" spans="1:17" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="28">
+        <v>6</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-    </row>
-    <row r="15" spans="1:46" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
-        <v>4</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="30" t="s">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+    </row>
+    <row r="18" spans="1:17" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="29">
+        <v>7</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+    </row>
+    <row r="19" spans="1:17" ht="34.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="30">
+        <v>8</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+    </row>
+    <row r="20" spans="1:17" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="30">
+        <v>9</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-    </row>
-    <row r="16" spans="1:46" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
-        <v>5</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="30" t="s">
+      <c r="C20" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-    </row>
-    <row r="17" spans="1:17" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>6</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="30" t="s">
+      <c r="D20" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+    </row>
+    <row r="21" spans="1:17" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="30">
+        <v>10</v>
+      </c>
+      <c r="B21" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-    </row>
-    <row r="18" spans="1:17" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19">
-        <v>7</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="27" t="s">
+      <c r="C21" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
+    </row>
+    <row r="22" spans="1:17" ht="40.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="30">
+        <v>11</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="25"/>
-    </row>
-    <row r="19" spans="1:17" ht="34.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22">
-        <v>8</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="27" t="s">
+      <c r="C22" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+    </row>
+    <row r="23" spans="1:17" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="30">
+        <v>12</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-    </row>
-    <row r="20" spans="1:17" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22">
-        <v>9</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-    </row>
-    <row r="21" spans="1:17" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22">
-        <v>10</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-    </row>
-    <row r="22" spans="1:17" ht="40.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22">
-        <v>11</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-    </row>
-    <row r="23" spans="1:17" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22">
-        <v>12</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
     </row>
     <row r="24" spans="1:17" ht="30.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="16"/>
+      <c r="B24" s="14"/>
     </row>
     <row r="25" spans="1:17" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="16"/>
+      <c r="B25" s="14"/>
     </row>
     <row r="26" spans="1:17" ht="34.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="16"/>
+      <c r="B26" s="14"/>
     </row>
     <row r="27" spans="1:17" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="16"/>
+      <c r="B27" s="14"/>
     </row>
     <row r="28" spans="1:17" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:17" ht="36.6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:17" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="17"/>
+      <c r="A31" s="15"/>
     </row>
     <row r="32" spans="1:17" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="17"/>
+      <c r="A32" s="15"/>
     </row>
     <row r="33" spans="1:18" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="17"/>
+      <c r="A33" s="15"/>
     </row>
     <row r="34" spans="1:18" ht="37.15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:18" ht="31.9" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1763,7 +1753,7 @@
     <row r="41" spans="1:18" ht="50.45" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:18" ht="41.45" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:18" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="R43" s="15"/>
+      <c r="R43" s="13"/>
     </row>
     <row r="44" spans="1:18" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>

<commit_message>
cap nhat lai cong viec tuan
</commit_message>
<xml_diff>
--- a/BangKeHoachLamViecNhom.xlsx
+++ b/BangKeHoachLamViecNhom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t>STT</t>
   </si>
@@ -171,9 +171,6 @@
     <t>Trần Văn Đồng, Trần Quang Đạo</t>
   </si>
   <si>
-    <t xml:space="preserve"> Trần Quang Đạo,Nguyễn Bùi Thiên Đạt</t>
-  </si>
-  <si>
     <t>Nguyễn Bùi Thiên Đạt, Trần Văn Đồng</t>
   </si>
   <si>
@@ -195,9 +192,6 @@
     <t>Viết thiết kế giao diện</t>
   </si>
   <si>
-    <t>Trần Văn Đồng</t>
-  </si>
-  <si>
     <t>TIMELINE THỰC HIỆN THIẾT KẾ HỆ THỐNG WEBSITE BÁN ĐIỆN THOẠI</t>
   </si>
   <si>
@@ -208,9 +202,6 @@
   </si>
   <si>
     <t>Viết thiết kế xử lý</t>
-  </si>
-  <si>
-    <t>Lý Gia Đào Trần Văn Đồng</t>
   </si>
 </sst>
 </file>
@@ -1050,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1083,7 +1074,7 @@
   <sheetData>
     <row r="1" spans="1:46" ht="61.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -1268,7 +1259,7 @@
         <v>33</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="11"/>
@@ -1291,7 +1282,7 @@
         <v>34</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="16"/>
@@ -1314,7 +1305,7 @@
         <v>35</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="16"/>
@@ -1341,7 +1332,7 @@
         <v>36</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="16"/>
@@ -1487,7 +1478,7 @@
         <v>42</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
@@ -1514,7 +1505,7 @@
         <v>43</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
@@ -1541,7 +1532,7 @@
         <v>44</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
@@ -1568,7 +1559,7 @@
         <v>45</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="21"/>
@@ -1595,7 +1586,7 @@
         <v>46</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
@@ -1616,13 +1607,13 @@
         <v>9</v>
       </c>
       <c r="B20" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>53</v>
-      </c>
       <c r="D20" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
@@ -1643,13 +1634,13 @@
         <v>10</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
@@ -1670,10 +1661,10 @@
         <v>11</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>21</v>
@@ -1697,13 +1688,13 @@
         <v>12</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>

</xml_diff>

<commit_message>
cap nhat cong viec
</commit_message>
<xml_diff>
--- a/BangKeHoachLamViecNhom.xlsx
+++ b/BangKeHoachLamViecNhom.xlsx
@@ -1031,7 +1031,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1041,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1701,8 +1701,8 @@
       <c r="G23" s="20"/>
       <c r="H23" s="20"/>
       <c r="I23" s="17"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="20"/>
       <c r="L23" s="9"/>
       <c r="M23" s="20"/>
       <c r="N23" s="17"/>

</xml_diff>